<commit_message>
Cross check accessibility guidlines, debug filtering logic
</commit_message>
<xml_diff>
--- a/assets/data/Cleaned_ALS_Website_Resource_MasterList_0409_2025.xlsx
+++ b/assets/data/Cleaned_ALS_Website_Resource_MasterList_0409_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/wtoh2_jh_edu/Documents/ALS Palliative Care Website Project/als-palliative-care-site/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="408" documentId="11_DFF5B153D46790CEEB3B98154B5DCE3A674BB37B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C10B497-76E5-49C9-979F-BFDBB300A53B}"/>
+  <xr:revisionPtr revIDLastSave="409" documentId="11_DFF5B153D46790CEEB3B98154B5DCE3A674BB37B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{472D92E6-696F-4959-B622-85EB3F1E565E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Website_Resources_Export" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="177">
   <si>
     <t>title</t>
   </si>
@@ -377,9 +377,6 @@
   </si>
   <si>
     <t>https://www.mda.org/alsn/article/not-gloom-and-doom-demystifying-hospice</t>
-  </si>
-  <si>
-    <t>Definition, Benefits/timing/who provides it</t>
   </si>
   <si>
     <t>https://www.roon.com/als/explore/palliative-care-PysUCeAcfQijStXYG3zBYs/end-of-life---hospice-CNzEULn6qEvqYxnzjsw2AE</t>
@@ -918,24 +915,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="113" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.1796875" customWidth="1"/>
-    <col min="2" max="2" width="58.36328125" customWidth="1"/>
-    <col min="3" max="3" width="34.6328125" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49.90625" customWidth="1"/>
+    <col min="1" max="1" width="48.21875" customWidth="1"/>
+    <col min="2" max="2" width="58.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.88671875" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="125.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="125.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -964,12 +961,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>48</v>
@@ -993,12 +990,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
@@ -1022,12 +1019,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>82</v>
@@ -1051,12 +1048,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
         <v>82</v>
@@ -1080,12 +1077,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
@@ -1109,12 +1106,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -1138,12 +1135,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -1167,12 +1164,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
         <v>82</v>
@@ -1196,12 +1193,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
         <v>48</v>
@@ -1225,12 +1222,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
         <v>48</v>
@@ -1254,12 +1251,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -1283,12 +1280,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
         <v>48</v>
@@ -1312,12 +1309,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
@@ -1338,15 +1335,15 @@
         <v>16</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C15" t="s">
         <v>43</v>
@@ -1370,12 +1367,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1399,12 +1396,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -1428,12 +1425,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
         <v>50</v>
@@ -1457,12 +1454,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
@@ -1486,12 +1483,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C20" t="s">
         <v>82</v>
@@ -1515,7 +1512,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1544,12 +1541,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
@@ -1570,15 +1567,15 @@
         <v>16</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
@@ -1599,15 +1596,15 @@
         <v>16</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
@@ -1631,12 +1628,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" t="s">
         <v>122</v>
-      </c>
-      <c r="B25" t="s">
-        <v>123</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
@@ -1645,10 +1642,10 @@
         <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
@@ -1657,15 +1654,15 @@
         <v>16</v>
       </c>
       <c r="I25" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
         <v>24</v>
@@ -1674,11 +1671,11 @@
         <v>10</v>
       </c>
       <c r="E26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" t="s">
         <v>124</v>
       </c>
-      <c r="F26" t="s">
-        <v>125</v>
-      </c>
       <c r="G26" t="s">
         <v>12</v>
       </c>
@@ -1686,15 +1683,15 @@
         <v>16</v>
       </c>
       <c r="I26" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C27" t="s">
         <v>48</v>
@@ -1703,10 +1700,10 @@
         <v>56</v>
       </c>
       <c r="E27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G27" t="s">
         <v>12</v>
@@ -1718,12 +1715,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C28" t="s">
         <v>48</v>
@@ -1732,10 +1729,10 @@
         <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
@@ -1744,15 +1741,15 @@
         <v>16</v>
       </c>
       <c r="I28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
@@ -1761,10 +1758,10 @@
         <v>56</v>
       </c>
       <c r="E29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
@@ -1776,12 +1773,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s">
         <v>36</v>
@@ -1790,27 +1787,27 @@
         <v>52</v>
       </c>
       <c r="E30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H30" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>111</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
         <v>48</v>
@@ -1819,10 +1816,10 @@
         <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F31" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
@@ -1834,12 +1831,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C32" t="s">
         <v>48</v>
@@ -1848,7 +1845,7 @@
         <v>83</v>
       </c>
       <c r="E32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F32" t="s">
         <v>58</v>
@@ -1863,12 +1860,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C33" t="s">
         <v>48</v>
@@ -1877,7 +1874,7 @@
         <v>83</v>
       </c>
       <c r="E33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
         <v>58</v>
@@ -1892,12 +1889,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C34" t="s">
         <v>43</v>
@@ -1906,7 +1903,7 @@
         <v>55</v>
       </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F34" t="s">
         <v>57</v>
@@ -1921,12 +1918,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C35" t="s">
         <v>48</v>
@@ -1935,7 +1932,7 @@
         <v>113</v>
       </c>
       <c r="E35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F35" t="s">
         <v>58</v>
@@ -1950,12 +1947,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -1964,7 +1961,7 @@
         <v>54</v>
       </c>
       <c r="E36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F36" t="s">
         <v>57</v>
@@ -1979,12 +1976,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -1993,7 +1990,7 @@
         <v>55</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F37" t="s">
         <v>58</v>
@@ -2008,7 +2005,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -2022,7 +2019,7 @@
         <v>56</v>
       </c>
       <c r="E38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F38" t="s">
         <v>58</v>
@@ -2037,12 +2034,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C39" t="s">
         <v>36</v>
@@ -2051,7 +2048,7 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F39" t="s">
         <v>58</v>
@@ -2063,15 +2060,15 @@
         <v>16</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C40" t="s">
         <v>48</v>
@@ -2095,12 +2092,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C41" t="s">
         <v>46</v>
@@ -2124,12 +2121,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
         <v>24</v>
@@ -2153,12 +2150,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C43" t="s">
         <v>48</v>
@@ -2182,12 +2179,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>35</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
         <v>36</v>
@@ -2211,12 +2208,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>30</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C45" t="s">
         <v>50</v>
@@ -2240,12 +2237,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C46" t="s">
         <v>48</v>
@@ -2269,12 +2266,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C47" t="s">
         <v>48</v>
@@ -2298,12 +2295,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
@@ -2327,12 +2324,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C49" t="s">
         <v>50</v>
@@ -2356,12 +2353,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C50" t="s">
         <v>43</v>
@@ -2385,12 +2382,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C51" t="s">
         <v>49</v>
@@ -2414,12 +2411,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>28</v>
       </c>
       <c r="B52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C52" t="s">
         <v>50</v>
@@ -2443,7 +2440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>32</v>
       </c>

</xml_diff>